<commit_message>
Data Processing for valuation engine
</commit_message>
<xml_diff>
--- a/asset/valuation_engine/Valuation_Engine_Mapping.xlsx
+++ b/asset/valuation_engine/Valuation_Engine_Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\valuation_engine\lookup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tao_project\dashboard_finance_metrics\asset\valuation_engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1074948D-36C6-493D-AA9E-6765F88B0B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B608A56-CD57-43E4-9142-B0FDBBB4EE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{DB505F9D-00EE-40BB-9331-63CC137490AC}"/>
   </bookViews>
@@ -27,12 +27,22 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Descending Helper'!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Formula!$A$1:$C$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Formula!$A$1:$E$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Industries!$A$1:$B$20</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -74,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="489">
   <si>
     <t>is.net_revenue</t>
   </si>
@@ -1414,6 +1424,135 @@
   </si>
   <si>
     <t>((q_df.loc[index,'cfs.cfo']+(q_df.loc[index,'is.interest_expense']*(1-q_df.loc[index,'is.income_tax_provision']/(q_df.loc[index,'is.income_tax_provision']+q_df.loc[index,'is.net_income'])))-abs(q_df.loc[index,'cfs.capital_expenditure']))-(q_df.loc[index-1,'cfs.cfo']+(q_df.loc[index-1,'is.interest_expense']*(1-q_df.loc[index-1,'is.income_tax_provision']/(q_df.loc[index-1,'is.income_tax_provision']+q_df.loc[index-1,'is.net_income'])))-abs(q_df.loc[index-1,'cfs.capital_expenditure'])))/abs((q_df.loc[index-1,'cfs.cfo']+(q_df.loc[index-1,'is.interest_expense']*(1-q_df.loc[index-1,'is.income_tax_provision']/(q_df.loc[index-1,'is.income_tax_provision']+q_df.loc[index-1,'is.net_income'])))-abs(q_df.loc[index-1,'cfs.capital_expenditure'])))</t>
+  </si>
+  <si>
+    <t>days_inventory_on_hand</t>
+  </si>
+  <si>
+    <t>days_sales_outstanding</t>
+  </si>
+  <si>
+    <t>days_payable</t>
+  </si>
+  <si>
+    <t>cash_conversion_cycle</t>
+  </si>
+  <si>
+    <t>working_capital_turnover</t>
+  </si>
+  <si>
+    <t>total_asset_turnover</t>
+  </si>
+  <si>
+    <t>quick_ratio</t>
+  </si>
+  <si>
+    <t>cash_ratio</t>
+  </si>
+  <si>
+    <t>debt_to_asset</t>
+  </si>
+  <si>
+    <t>debt_to_capital</t>
+  </si>
+  <si>
+    <t>debt_to_equity</t>
+  </si>
+  <si>
+    <t>financial_leverage</t>
+  </si>
+  <si>
+    <t>interest_coverage</t>
+  </si>
+  <si>
+    <t>interest_ratio</t>
+  </si>
+  <si>
+    <t>gross_profit_margin</t>
+  </si>
+  <si>
+    <t>operating_profit_margin</t>
+  </si>
+  <si>
+    <t>ebitda_margin</t>
+  </si>
+  <si>
+    <t>net_profit_margin</t>
+  </si>
+  <si>
+    <t>return_on_asset</t>
+  </si>
+  <si>
+    <t>return_on_equity</t>
+  </si>
+  <si>
+    <t>depreciation_ratio</t>
+  </si>
+  <si>
+    <t>cash_growth_rate</t>
+  </si>
+  <si>
+    <t>debt_growth_rate</t>
+  </si>
+  <si>
+    <t>outstanding_shares_growth_rate</t>
+  </si>
+  <si>
+    <t>inventory_growth_rate</t>
+  </si>
+  <si>
+    <t>pp&amp;e_growth_rate</t>
+  </si>
+  <si>
+    <t>goodwill_growth_rate</t>
+  </si>
+  <si>
+    <t>total_asset_growth_rate</t>
+  </si>
+  <si>
+    <t>sg_a_ratio</t>
+  </si>
+  <si>
+    <t>r_d_ratio</t>
+  </si>
+  <si>
+    <t>revenue_growth_rate</t>
+  </si>
+  <si>
+    <t>return_on_invested_capital_rate</t>
+  </si>
+  <si>
+    <t>eps_growth_rate</t>
+  </si>
+  <si>
+    <t>adj_equity_growth_rate</t>
+  </si>
+  <si>
+    <t>free_cashflow_growth_rate</t>
+  </si>
+  <si>
+    <t>Formula_Shortname</t>
+  </si>
+  <si>
+    <t>Formula_Category</t>
+  </si>
+  <si>
+    <t>Efficiency Ratio</t>
+  </si>
+  <si>
+    <t>Liquidity Ratio</t>
+  </si>
+  <si>
+    <t>Solvency Ratio</t>
+  </si>
+  <si>
+    <t>Profitability Ratio</t>
+  </si>
+  <si>
+    <t>Miscellaneous Ratio</t>
+  </si>
+  <si>
+    <t>Key Ratio</t>
   </si>
 </sst>
 </file>
@@ -1421,7 +1560,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1497,11 +1636,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3339,7 +3478,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3358,45 +3497,45 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B2" t="s">
-        <v>433</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>169</v>
+      </c>
+      <c r="B8" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3406,42 +3545,42 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -3451,10 +3590,15 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B20" xr:uid="{5FF8DD67-EF32-46CE-967F-FCAE0BBB8B6E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
+      <sortCondition ref="A1:A20"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3462,19 +3606,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6085D-466B-40F3-BD6F-CEE4B7C0DEBD}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>202</v>
       </c>
@@ -3484,8 +3632,14 @@
       <c r="C1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>481</v>
+      </c>
+      <c r="E1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>204</v>
       </c>
@@ -3495,8 +3649,14 @@
       <c r="C2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>476</v>
+      </c>
+      <c r="E2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>206</v>
       </c>
@@ -3506,8 +3666,14 @@
       <c r="C3" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>477</v>
+      </c>
+      <c r="E3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>208</v>
       </c>
@@ -3517,8 +3683,14 @@
       <c r="C4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>478</v>
+      </c>
+      <c r="E4" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>209</v>
       </c>
@@ -3528,8 +3700,14 @@
       <c r="C5" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>479</v>
+      </c>
+      <c r="E5" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>210</v>
       </c>
@@ -3539,8 +3717,14 @@
       <c r="C6" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>480</v>
+      </c>
+      <c r="E6" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>211</v>
       </c>
@@ -3550,8 +3734,14 @@
       <c r="C7" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>446</v>
+      </c>
+      <c r="E7" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>212</v>
       </c>
@@ -3561,8 +3751,14 @@
       <c r="C8" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>447</v>
+      </c>
+      <c r="E8" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -3572,8 +3768,14 @@
       <c r="C9" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>448</v>
+      </c>
+      <c r="E9" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>214</v>
       </c>
@@ -3583,8 +3785,14 @@
       <c r="C10" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>449</v>
+      </c>
+      <c r="E10" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>215</v>
       </c>
@@ -3594,8 +3802,14 @@
       <c r="C11" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>450</v>
+      </c>
+      <c r="E11" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>216</v>
       </c>
@@ -3605,8 +3819,14 @@
       <c r="C12" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>451</v>
+      </c>
+      <c r="E12" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -3616,8 +3836,14 @@
       <c r="C13" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>452</v>
+      </c>
+      <c r="E13" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>218</v>
       </c>
@@ -3627,8 +3853,14 @@
       <c r="C14" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>453</v>
+      </c>
+      <c r="E14" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>219</v>
       </c>
@@ -3638,8 +3870,14 @@
       <c r="C15" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>454</v>
+      </c>
+      <c r="E15" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>220</v>
       </c>
@@ -3649,8 +3887,14 @@
       <c r="C16" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>455</v>
+      </c>
+      <c r="E16" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>221</v>
       </c>
@@ -3660,8 +3904,14 @@
       <c r="C17" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>456</v>
+      </c>
+      <c r="E17" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>222</v>
       </c>
@@ -3671,8 +3921,14 @@
       <c r="C18" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>457</v>
+      </c>
+      <c r="E18" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>223</v>
       </c>
@@ -3682,8 +3938,14 @@
       <c r="C19" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>458</v>
+      </c>
+      <c r="E19" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>224</v>
       </c>
@@ -3693,8 +3955,14 @@
       <c r="C20" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>459</v>
+      </c>
+      <c r="E20" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>225</v>
       </c>
@@ -3704,8 +3972,14 @@
       <c r="C21" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>460</v>
+      </c>
+      <c r="E21" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>226</v>
       </c>
@@ -3715,8 +3989,14 @@
       <c r="C22" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>461</v>
+      </c>
+      <c r="E22" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>227</v>
       </c>
@@ -3726,8 +4006,14 @@
       <c r="C23" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>462</v>
+      </c>
+      <c r="E23" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>228</v>
       </c>
@@ -3737,8 +4023,14 @@
       <c r="C24" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>463</v>
+      </c>
+      <c r="E24" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>229</v>
       </c>
@@ -3748,8 +4040,14 @@
       <c r="C25" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>464</v>
+      </c>
+      <c r="E25" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>230</v>
       </c>
@@ -3759,8 +4057,14 @@
       <c r="C26" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>465</v>
+      </c>
+      <c r="E26" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>231</v>
       </c>
@@ -3770,8 +4074,14 @@
       <c r="C27" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>474</v>
+      </c>
+      <c r="E27" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>232</v>
       </c>
@@ -3781,8 +4091,14 @@
       <c r="C28" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>475</v>
+      </c>
+      <c r="E28" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>233</v>
       </c>
@@ -3792,8 +4108,14 @@
       <c r="C29" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>466</v>
+      </c>
+      <c r="E29" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>234</v>
       </c>
@@ -3803,8 +4125,14 @@
       <c r="C30" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>467</v>
+      </c>
+      <c r="E30" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>235</v>
       </c>
@@ -3814,8 +4142,14 @@
       <c r="C31" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>468</v>
+      </c>
+      <c r="E31" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>236</v>
       </c>
@@ -3825,8 +4159,14 @@
       <c r="C32" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>469</v>
+      </c>
+      <c r="E32" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>237</v>
       </c>
@@ -3836,8 +4176,14 @@
       <c r="C33" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>470</v>
+      </c>
+      <c r="E33" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>238</v>
       </c>
@@ -3847,8 +4193,14 @@
       <c r="C34" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>471</v>
+      </c>
+      <c r="E34" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>239</v>
       </c>
@@ -3858,8 +4210,14 @@
       <c r="C35" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>472</v>
+      </c>
+      <c r="E35" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>240</v>
       </c>
@@ -3869,9 +4227,15 @@
       <c r="C36" t="s">
         <v>284</v>
       </c>
+      <c r="D36" t="s">
+        <v>473</v>
+      </c>
+      <c r="E36" t="s">
+        <v>487</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C36" xr:uid="{F4D6085D-466B-40F3-BD6F-CEE4B7C0DEBD}"/>
+  <autoFilter ref="A1:E36" xr:uid="{F4D6085D-466B-40F3-BD6F-CEE4B7C0DEBD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>